<commit_message>
multipl purchase price for product
</commit_message>
<xml_diff>
--- a/assets/sample_files/Item Detail.xlsx
+++ b/assets/sample_files/Item Detail.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\www\tiles\assets\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\tiles_project\assets\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA4B537-2CD4-4A83-BC51-718FCE409093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24B6DA02-7501-402A-AE29-1CD90CD133A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Quantity</t>
   </si>
@@ -103,12 +102,18 @@
   </si>
   <si>
     <t>wall tiles</t>
+  </si>
+  <si>
+    <t>2000 , 200 , 1000</t>
+  </si>
+  <si>
+    <t>15 , 10 , 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3301C5B3-D879-4923-BE1F-F2EA1DB95DF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,9 +516,9 @@
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -585,14 +590,14 @@
       <c r="G2" s="6">
         <v>2</v>
       </c>
-      <c r="H2" s="6">
-        <v>2000</v>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="6">
-        <v>15</v>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="K2" s="1">
         <v>0.82</v>

</xml_diff>

<commit_message>
calculation of qunatity per unit in history table
</commit_message>
<xml_diff>
--- a/assets/sample_files/Item Detail.xlsx
+++ b/assets/sample_files/Item Detail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Quantity</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>factor</t>
-  </si>
-  <si>
-    <t>Quantity Per Unit</t>
   </si>
   <si>
     <t>Item Group</t>
@@ -502,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,11 +517,10 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -562,13 +558,10 @@
         <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -591,57 +584,54 @@
         <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1">
         <v>0.82</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1">
         <v>1550</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="P4" s="7" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O4" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q5" s="3" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q6" s="3" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q7" s="3" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q8" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="O4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Task_1 in PNPTiles Completed
</commit_message>
<xml_diff>
--- a/assets/sample_files/Item Detail.xlsx
+++ b/assets/sample_files/Item Detail.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\www\tiles\assets\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\tiles_project\assets\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA4B537-2CD4-4A83-BC51-718FCE409093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24B6DA02-7501-402A-AE29-1CD90CD133A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Quantity</t>
   </si>
@@ -96,19 +95,22 @@
     <t>factor</t>
   </si>
   <si>
-    <t>Quantity Per Unit</t>
-  </si>
-  <si>
     <t>Item Group</t>
   </si>
   <si>
     <t>wall tiles</t>
+  </si>
+  <si>
+    <t>2000 , 200 , 1000</t>
+  </si>
+  <si>
+    <t>15 , 10 , 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,11 +498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3301C5B3-D879-4923-BE1F-F2EA1DB95DF9}">
-  <dimension ref="A1:R8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,15 +513,14 @@
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -557,13 +558,10 @@
         <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -585,58 +583,55 @@
       <c r="G2" s="6">
         <v>2</v>
       </c>
-      <c r="H2" s="6">
-        <v>2000</v>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="6">
-        <v>15</v>
+      <c r="J2" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="K2" s="1">
         <v>0.82</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1">
         <v>1550</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="P4" s="7" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O4" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q5" s="3" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q6" s="3" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q7" s="3" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q8" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="O4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>